<commit_message>
updated template with colo schema
</commit_message>
<xml_diff>
--- a/template/SPA/country_data.xlsx
+++ b/template/SPA/country_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/template/SPA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47574F8E-3CD3-624B-9893-8F1E463E25B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD6C748-CC49-6844-914C-F932754D2675}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30240" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="4" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" activeTab="6" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
     <sheet name="6-Brotes de EPV" sheetId="6" r:id="rId6"/>
     <sheet name="Glosario" sheetId="7" r:id="rId7"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId8"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -326,7 +323,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -382,13 +379,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -403,8 +393,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -424,31 +427,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFBDBB5"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFDF59B"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB3C5DB"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC4B5D9"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -801,7 +828,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -810,15 +837,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -834,35 +854,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -878,35 +898,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -918,7 +938,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -927,64 +947,104 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1004,42 +1064,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="1-General"/>
-      <sheetName val="2-Área pop "/>
-      <sheetName val="3-Inmunidad poblacional"/>
-      <sheetName val="4-Desempeño del programa "/>
-      <sheetName val="5-Grupos vulnerables"/>
-      <sheetName val="6-Datos caso a caso"/>
-      <sheetName val="7-Respuesta rápida"/>
-      <sheetName val="_ListValues"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="3">
-          <cell r="B3">
-            <v>2023</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1430,7 +1454,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1443,63 +1467,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="9"/>
+      <c r="A2" s="59"/>
+      <c r="B2" s="59"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="9"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="9"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="9"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1510,8 +1534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87362FD8-F1C8-0142-963D-AD6273C5898D}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1526,157 +1550,152 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="49" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="45" t="s">
+      <c r="G1" s="53" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="45"/>
-      <c r="I1" s="45"/>
-      <c r="J1" s="45"/>
-      <c r="K1" s="45"/>
-      <c r="L1" s="45" t="s">
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="53" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="42" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="5">
-        <f>'[1]1-General'!$B$3-5</f>
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="55">
         <v>2018</v>
       </c>
-      <c r="H2" s="5">
-        <f>'[1]1-General'!$B$3-4</f>
+      <c r="H2" s="55">
         <v>2019</v>
       </c>
-      <c r="I2" s="5">
-        <f>'[1]1-General'!$B$3-3</f>
+      <c r="I2" s="55">
         <v>2020</v>
       </c>
-      <c r="J2" s="5">
-        <f>'[1]1-General'!$B$3-2</f>
+      <c r="J2" s="55">
         <v>2021</v>
       </c>
-      <c r="K2" s="5">
-        <f>'[1]1-General'!$B$3-1</f>
+      <c r="K2" s="55">
         <v>2022</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1703,8 +1722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24FC60A-8114-B04C-B5D4-941061AFF1F9}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1719,156 +1738,156 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="64" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="52" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="H1" s="64" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="5" t="s">
+      <c r="I1" s="65"/>
+      <c r="J1" s="65"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="63" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="91" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="5" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="63" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="63" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1893,8 +1912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CC216D-4B82-884B-A94C-AD4D5EE82E42}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1903,104 +1922,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="47" t="s">
+      <c r="E1" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="47" t="s">
+      <c r="F1" s="66" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="76" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="76" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="5" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="76" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -2025,7 +2044,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2034,112 +2053,112 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="45" t="s">
+      <c r="D1" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="71" t="s">
         <v>34</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
     </row>
     <row r="2" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="49"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="5" t="s">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="73" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="59"/>
+      <c r="B3" s="59"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="59"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="59"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="6"/>
-      <c r="B6" s="6"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="6"/>
-      <c r="B7" s="6"/>
+      <c r="A7" s="59"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
-      <c r="B8" s="6"/>
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2162,369 +2181,369 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24261340-693F-D844-8FDC-79D93DCEE3FF}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="44" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="42" customWidth="1"/>
     <col min="3" max="3" width="27.1640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="10" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+      <c r="A2" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="61"/>
-      <c r="B3" s="41" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26"/>
-      <c r="E3" s="27"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="61"/>
-      <c r="B4" s="34" t="s">
+      <c r="A4" s="47"/>
+      <c r="B4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="61"/>
-      <c r="B5" s="41" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="27"/>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="62"/>
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="48"/>
+      <c r="B6" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="26"/>
     </row>
     <row r="7" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A7" s="63" t="s">
+      <c r="A7" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="31" t="s">
+      <c r="E7" s="29" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="64"/>
-      <c r="B8" s="19" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="E8" s="18"/>
+      <c r="E8" s="16"/>
     </row>
     <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A9" s="64"/>
-      <c r="B9" s="19" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="20" t="s">
+      <c r="E9" s="18" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
-      <c r="B10" s="22" t="s">
+      <c r="A10" s="51"/>
+      <c r="B10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="33" t="s">
+      <c r="E10" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A11" s="52" t="s">
+      <c r="A11" s="60" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="61"/>
+      <c r="B12" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="19" t="s">
+      <c r="D12" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
-      <c r="B13" s="19" t="s">
+      <c r="A13" s="61"/>
+      <c r="B13" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="19" t="s">
+      <c r="C13" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A14" s="53"/>
-      <c r="B14" s="19" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
-      <c r="B15" s="19" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="C15" s="19" t="s">
+      <c r="C15" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="19" t="s">
+      <c r="D15" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-      <c r="B16" s="19" t="s">
+      <c r="A16" s="61"/>
+      <c r="B16" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="19" t="s">
+      <c r="C16" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="19" t="s">
+      <c r="D16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="18" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="54"/>
-      <c r="B17" s="35" t="s">
+      <c r="A17" s="62"/>
+      <c r="B17" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="34" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="160" x14ac:dyDescent="0.2">
-      <c r="A18" s="55" t="s">
+      <c r="A18" s="74" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="19" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="113" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="56"/>
-      <c r="B19" s="32" t="s">
+      <c r="A19" s="75"/>
+      <c r="B19" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" s="31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="68" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="16"/>
+      <c r="E20" s="14"/>
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="58"/>
-      <c r="B21" s="38" t="s">
+      <c r="A21" s="69"/>
+      <c r="B21" s="36" t="s">
         <v>80</v>
       </c>
-      <c r="C21" s="19" t="s">
+      <c r="C21" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E21" s="18"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="58"/>
-      <c r="B22" s="38" t="s">
+      <c r="A22" s="69"/>
+      <c r="B22" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="58"/>
-      <c r="B23" s="38" t="s">
+      <c r="A23" s="69"/>
+      <c r="B23" s="36" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="E23" s="18"/>
+      <c r="E23" s="16"/>
     </row>
     <row r="24" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="59"/>
-      <c r="B24" s="32" t="s">
+      <c r="A24" s="70"/>
+      <c r="B24" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="E24" s="23"/>
+      <c r="E24" s="21"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="B25" s="43"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
+      <c r="B25" s="41"/>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
feat: spanish, english and french country_data template
</commit_message>
<xml_diff>
--- a/template/SPA/country_data.xlsx
+++ b/template/SPA/country_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivermazariegos/Sites/polio-risk/template/SPA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://paho-my.sharepoint.com/personal/caine_paho_org/Documents/WDC/Polio/2023/AR municipal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E196B26F-D9A3-094C-8416-36E1B5628998}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{689AE1EB-FEA6-49E5-9577-E48F78BB7934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E65D68E9-2FE5-4F6D-80A5-874ACCC38B68}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="760" windowWidth="25020" windowHeight="18880" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14660" firstSheet="1" activeTab="6" xr2:uid="{7CFA64C4-648F-B840-901A-EC2D94882293}"/>
   </bookViews>
   <sheets>
     <sheet name="1-General" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="101">
   <si>
     <t>Datos generales</t>
   </si>
@@ -84,267 +84,270 @@
     <t>Cobertura administrativa de Polio 3 por municipio</t>
   </si>
   <si>
-    <t>Porcentaje de cobertura con IPV2 2022</t>
-  </si>
-  <si>
-    <t>¿Si el país llevó a cabo una campaña de vacunación contra la polio en 2018-2022, se alcanzó una cobertura &gt;95% en el municipio?</t>
-  </si>
-  <si>
     <t>Unidades Notificadoras</t>
   </si>
   <si>
-    <t>% de unidades notificadoras que enviaron información en todas las semanas durante el periodo evaluado (2022)</t>
+    <t>Tasa PFA</t>
+  </si>
+  <si>
+    <t>% de casos de PFA con notificación oportuna (antes de 14 días desde el inicio de la parálisis)</t>
+  </si>
+  <si>
+    <t>% de casos de PFA investigados en menos de 48 horas</t>
+  </si>
+  <si>
+    <t>% de casos con muestra adecuada de heces</t>
+  </si>
+  <si>
+    <t>% de casos con seguimiento a los 60 días</t>
+  </si>
+  <si>
+    <t>¿En los municipios con &lt;100000 menores de 15 años y que no presentaron casos de PFA, se llevaron a cabo búsquedas activas institucionales en al menos un establecimiento de salud del municipio?</t>
+  </si>
+  <si>
+    <t>Población con acceso a servicios básicos de agua potable</t>
+  </si>
+  <si>
+    <t>% de la población con acceso a servicios básicos de agua potable</t>
+  </si>
+  <si>
+    <t>Población con acceso a servicios básicos de saneamiento</t>
+  </si>
+  <si>
+    <t>% de la población con acceso a servicios básicos de saneamiento</t>
+  </si>
+  <si>
+    <t>Presencia de brotes en los últimos 5 años</t>
+  </si>
+  <si>
+    <t>Sarampión</t>
+  </si>
+  <si>
+    <t>Difteria</t>
+  </si>
+  <si>
+    <t>Fiebre amarilla</t>
+  </si>
+  <si>
+    <t>Hoja</t>
+  </si>
+  <si>
+    <t>Celda</t>
+  </si>
+  <si>
+    <t>Definición</t>
+  </si>
+  <si>
+    <t>Tipo de información</t>
+  </si>
+  <si>
+    <t>Notas</t>
+  </si>
+  <si>
+    <t>Dependiendo del país, se debe introducir el nombre de la región, departamento o estado.</t>
+  </si>
+  <si>
+    <t>Texto</t>
+  </si>
+  <si>
+    <t>Nombre del municipio.</t>
+  </si>
+  <si>
+    <t>Número de menores de 15 años de edad en el municipio.</t>
+  </si>
+  <si>
+    <t>Número</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seleccione Si o No </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esta celda cambiará a gris para los municipios con menos de 100000 menores de 15 años de edad. No es necesario completar la información en estos casos pero puede seleccionar NA si lo desea. </t>
+  </si>
+  <si>
+    <t>Cobertura administrativa para Polio3 para el año correspondiente</t>
+  </si>
+  <si>
+    <t>Si IPV2 no ha sido introducida, coloque 0 (cero)</t>
+  </si>
+  <si>
+    <t>Seleccione Si, No o NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Si el país no tuvo campañas de vacunación contra la polio, seleccione NA. Si se llevaron a cabo múltiples campañas, seleccione la cobertura de la campaña más reciente. </t>
+  </si>
+  <si>
+    <t>Vigilancia</t>
+  </si>
+  <si>
+    <t>Porcentaje de unidades notificadoras que enviaron información en todas las semanas del años.</t>
+  </si>
+  <si>
+    <t>Si el municipio no tiene unidades notificadoras, se debe colocar cero.</t>
+  </si>
+  <si>
+    <t>Tasa de PFA</t>
+  </si>
+  <si>
+    <t>Porcentaje de casos de PFA que fueron reportados antes de 14 días del inicio de la parálisis.</t>
+  </si>
+  <si>
+    <t>Porcentaje de casos de PFA que fueron investigados en menos de 48 horas a partir del reporte.</t>
+  </si>
+  <si>
+    <t>% de casos de PFA con muestra adecuada de heces</t>
+  </si>
+  <si>
+    <t>Porcentaje de casos de PFA con muestra adecuada de heces.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porcentaje de casos de PFA con seguimiento a los 60 días. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">En los municipios con menos de 100000 menores de 15 años y que no presentaron casos de PFA, determine si se llevaron a cabo búsquedas activas institucionales en al menos un establecimiento de salud del municipio. </t>
+  </si>
+  <si>
+    <t>Determinantes</t>
+  </si>
+  <si>
+    <t>Porcentaje de la población con acceso a servicios básicos de agua potable. El acceso a servicios básicos de agua potable se define como acceso a agua potable de una fuente mejorada, siempre que el tiempo de recolección no sea superior a 30 minutos en el recorrido de ida y vuelta, incluido el tiempo de espera en filas.*</t>
+  </si>
+  <si>
+    <t>Si no se conoce el porcentaje, se puede poner un estimado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porcentaje de la población con acceso a servicios básicos de saneamiento. Los servicios básicos de saneamiento se refieren al uso de instalaciones mejoradas que no se comparten con otros hogares.* </t>
+  </si>
+  <si>
+    <t>El municipio tuvo casos de sarampión  en los últimos 5 años.</t>
+  </si>
+  <si>
+    <t>Rubéola</t>
+  </si>
+  <si>
+    <t>El municipio tuvo casos de rubéola en los últimos 5 años.</t>
+  </si>
+  <si>
+    <t>El municipio tuvo casos de difteria en los últimos 5 años.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">El municipio tuvo casos de fiebre amarilla en los últimos 5 años. </t>
+  </si>
+  <si>
+    <t>Tétanos neonatal</t>
+  </si>
+  <si>
+    <t>El municipio tuvo casos de tétanos neonatal en los útlimos 5 años.</t>
+  </si>
+  <si>
+    <t>* Definición de "La Agenda 2020 para el abastecimiento de agua, el sanemaiento y la higiene en América Latina y el Caribe" disponible en https://iris.paho.org/handle/10665.2/51836</t>
+  </si>
+  <si>
+    <t>Area poblacional</t>
+  </si>
+  <si>
+    <t>Inmunidad poblacional</t>
+  </si>
+  <si>
+    <t>Brotes de EPV</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Yes No</t>
+  </si>
+  <si>
+    <t>Outbreaks</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Población &lt;5 años de edad</t>
+  </si>
+  <si>
+    <t>Población &lt;1 año de edad</t>
+  </si>
+  <si>
+    <t>Polio</t>
+  </si>
+  <si>
+    <t>Número de menores de 1 años de edad en el municipio.</t>
+  </si>
+  <si>
+    <t>Número de menores de 5 años de edad en el municipio.</t>
+  </si>
+  <si>
+    <t>Número total de municipios</t>
+  </si>
+  <si>
+    <t>Esquema de vacunación contra la polio</t>
+  </si>
+  <si>
+    <t>Población total</t>
+  </si>
+  <si>
+    <t>¿Si la población &lt;15 años de edad es &lt;100000, se presentaron casos de PFA en el 2023?</t>
+  </si>
+  <si>
+    <t>Porcentaje de cobertura con IPV2 2023</t>
+  </si>
+  <si>
+    <t>¿Si el país llevó a cabo una campaña de vacunación contra la polio en 2019-2023, se alcanzó una cobertura &gt;95% en el municipio?</t>
+  </si>
+  <si>
+    <t>% de unidades notificadoras que enviaron información en todas las semanas durante el periodo evaluado (2023)</t>
   </si>
   <si>
     <t>Vigilancia de las PFA 
-(para municipios con &gt;100000 menores de 15 años O municipios con &lt;100000 menores de 15 años que tuvieron casos de PFA en el 2022)</t>
-  </si>
-  <si>
-    <t>Tasa PFA</t>
-  </si>
-  <si>
-    <t>% de casos de PFA con notificación oportuna (antes de 14 días desde el inicio de la parálisis)</t>
-  </si>
-  <si>
-    <t>% de casos de PFA investigados en menos de 48 horas</t>
-  </si>
-  <si>
-    <t>% de casos con muestra adecuada de heces</t>
-  </si>
-  <si>
-    <t>% de casos con seguimiento a los 60 días</t>
+(para municipios con &gt;100000 menores de 15 años O municipios con &lt;100000 menores de 15 años que tuvieron casos de PFA en el 2023)</t>
   </si>
   <si>
     <t>Búsqueda activa institucional
-(para municipios con &lt;100000 menores de 15 años SIN casos de PFA en el 2022)</t>
-  </si>
-  <si>
-    <t>¿En los municipios con &lt;100000 menores de 15 años y que no presentaron casos de PFA, se llevaron a cabo búsquedas activas institucionales en al menos un establecimiento de salud del municipio?</t>
-  </si>
-  <si>
-    <t>Población con acceso a servicios básicos de agua potable</t>
-  </si>
-  <si>
-    <t>% de la población con acceso a servicios básicos de agua potable</t>
-  </si>
-  <si>
-    <t>Población con acceso a servicios básicos de saneamiento</t>
-  </si>
-  <si>
-    <t>% de la población con acceso a servicios básicos de saneamiento</t>
-  </si>
-  <si>
-    <t>Presencia de brotes en los últimos 5 años</t>
-  </si>
-  <si>
-    <t>Sarampión</t>
-  </si>
-  <si>
-    <t>Rubiola</t>
-  </si>
-  <si>
-    <t>Difteria</t>
-  </si>
-  <si>
-    <t>Fiebre amarilla</t>
-  </si>
-  <si>
-    <t>Tétano neonatal</t>
-  </si>
-  <si>
-    <t>Hoja</t>
-  </si>
-  <si>
-    <t>Celda</t>
-  </si>
-  <si>
-    <t>Definición</t>
-  </si>
-  <si>
-    <t>Tipo de información</t>
-  </si>
-  <si>
-    <t>Notas</t>
-  </si>
-  <si>
-    <t>Dependiendo del país, se debe introducir el nombre de la región, departamento o estado.</t>
-  </si>
-  <si>
-    <t>Texto</t>
-  </si>
-  <si>
-    <t>Nombre del municipio.</t>
-  </si>
-  <si>
-    <t>Número de menores de 15 años de edad en el municipio.</t>
-  </si>
-  <si>
-    <t>Número</t>
-  </si>
-  <si>
-    <t>¿Si la población &lt;15 años de edad es &lt;100000, se presentaron casos de PFA en el 2022?</t>
-  </si>
-  <si>
-    <t>Para los municipios con menos de 100000 menores de 15 años, determine si se presentaron casos de PFA en el 2022.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seleccione Si o No </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta celda cambiará a gris para los municipios con menos de 100000 menores de 15 años de edad. No es necesario completar la información en estos casos pero puede seleccionar NA si lo desea. </t>
-  </si>
-  <si>
-    <t>Cob. Adm. Polio3 2018, 2019, 2020, 2021 y 2022</t>
-  </si>
-  <si>
-    <t>Cobertura administrativa para Polio3 para el año correspondiente</t>
-  </si>
-  <si>
-    <t>Cobertura IPV2 2022</t>
-  </si>
-  <si>
-    <t>Cobertura administrativa para IPV2 en el 2022</t>
-  </si>
-  <si>
-    <t>Si IPV2 no ha sido introducida, coloque 0 (cero)</t>
-  </si>
-  <si>
-    <t>Para los países en los que se llevó a cabo una campaña de vacunación contra la polio entre 2018 y 2022, defina si la cobertura alcanzada en el municipio fue &gt;95%</t>
-  </si>
-  <si>
-    <t>Seleccione Si, No o NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Si el país no tuvo campañas de vacunación contra la polio, seleccione NA. Si se llevaron a cabo múltiples campañas, seleccione la cobertura de la campaña más reciente. </t>
-  </si>
-  <si>
-    <t>Vigilancia</t>
-  </si>
-  <si>
-    <t>Porcentaje de unidades notificadoras que enviaron información en todas las semanas del años.</t>
-  </si>
-  <si>
-    <t>Si el municipio no tiene unidades notificadoras, se debe colocar cero.</t>
-  </si>
-  <si>
-    <t>Tasa de PFA</t>
-  </si>
-  <si>
-    <t>Tasa de PFA para el municipio en 2022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Esta celda solo debe completarse para los municipios con &gt;100000 menores de 15 años o municipios con &lt;100000 pero que hayan tenido casos de PFA en el 2022. Para los municipios con &lt;100000 menores de 15 años y que no tuvieron casos de PFA en 2022, la celda cambiará a gris y no es necesario completar ninguna información. </t>
-  </si>
-  <si>
-    <t>Porcentaje de casos de PFA que fueron reportados antes de 14 días del inicio de la parálisis.</t>
-  </si>
-  <si>
-    <t>Porcentaje de casos de PFA que fueron investigados en menos de 48 horas a partir del reporte.</t>
-  </si>
-  <si>
-    <t>% de casos de PFA con muestra adecuada de heces</t>
-  </si>
-  <si>
-    <t>Porcentaje de casos de PFA con muestra adecuada de heces.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de casos de PFA con seguimiento a los 60 días. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">En los municipios con menos de 100000 menores de 15 años y que no presentaron casos de PFA, determine si se llevaron a cabo búsquedas activas institucionales en al menos un establecimiento de salud del municipio. </t>
-  </si>
-  <si>
-    <t>Esta celda solo debe completarse para los municipios con &lt;100000 menores de 15 años y que no hayan tenido casos de PFA en el 2022</t>
-  </si>
-  <si>
-    <t>Determinantes</t>
-  </si>
-  <si>
-    <t>Porcentaje de la población con acceso a servicios básicos de agua potable. El acceso a servicios básicos de agua potable se define como acceso a agua potable de una fuente mejorada, siempre que el tiempo de recolección no sea superior a 30 minutos en el recorrido de ida y vuelta, incluido el tiempo de espera en filas.*</t>
-  </si>
-  <si>
-    <t>Si no se conoce el porcentaje, se puede poner un estimado</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Porcentaje de la población con acceso a servicios básicos de saneamiento. Los servicios básicos de saneamiento se refieren al uso de instalaciones mejoradas que no se comparten con otros hogares.* </t>
-  </si>
-  <si>
-    <t>El municipio tuvo casos de sarampión  en los últimos 5 años.</t>
-  </si>
-  <si>
-    <t>Rubéola</t>
-  </si>
-  <si>
-    <t>El municipio tuvo casos de rubéola en los últimos 5 años.</t>
-  </si>
-  <si>
-    <t>El municipio tuvo casos de difteria en los últimos 5 años.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">El municipio tuvo casos de fiebre amarilla en los últimos 5 años. </t>
-  </si>
-  <si>
-    <t>Tétanos neonatal</t>
-  </si>
-  <si>
-    <t>El municipio tuvo casos de tétanos neonatal en los útlimos 5 años.</t>
-  </si>
-  <si>
-    <t>* Definición de "La Agenda 2020 para el abastecimiento de agua, el sanemaiento y la higiene en América Latina y el Caribe" disponible en https://iris.paho.org/handle/10665.2/51836</t>
-  </si>
-  <si>
-    <t>Area poblacional</t>
-  </si>
-  <si>
-    <t>Inmunidad poblacional</t>
-  </si>
-  <si>
-    <t>Brotes de EPV</t>
-  </si>
-  <si>
-    <t>Sex</t>
-  </si>
-  <si>
-    <t>Yes No</t>
-  </si>
-  <si>
-    <t>Outbreaks</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
-  <si>
-    <t>Si</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>Población &lt;5 años de edad</t>
-  </si>
-  <si>
-    <t>Población &lt;1 año de edad</t>
-  </si>
-  <si>
-    <t>Polio</t>
-  </si>
-  <si>
-    <t>Número de menores de 1 años de edad en el municipio.</t>
-  </si>
-  <si>
-    <t>Número de menores de 5 años de edad en el municipio.</t>
-  </si>
-  <si>
-    <t>Número total de municipios</t>
-  </si>
-  <si>
-    <t>Guatemala</t>
-  </si>
-  <si>
-    <t>Esquema de vacunación contra la polio</t>
-  </si>
-  <si>
-    <t>Población total</t>
+(para municipios con &lt;100000 menores de 15 años SIN casos de PFA en el 2023)</t>
+  </si>
+  <si>
+    <t>Cob. Adm. Polio3 2019, 2020, 2021, 2022 y 2023</t>
+  </si>
+  <si>
+    <t>Cobertura IPV2 2023</t>
+  </si>
+  <si>
+    <t>Para los municipios con menos de 100000 menores de 15 años, determine si se presentaron casos de PFA en el 2023.</t>
+  </si>
+  <si>
+    <t>Cobertura administrativa para IPV2 en el 2023</t>
+  </si>
+  <si>
+    <t>Para los países en los que se llevó a cabo una campaña de vacunación contra la polio entre 2019 y 2023, defina si la cobertura alcanzada en el municipio fue &gt;95%</t>
+  </si>
+  <si>
+    <t>Tasa de PFA para el municipio en 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Esta celda solo debe completarse para los municipios con &gt;100000 menores de 15 años o municipios con &lt;100000 pero que hayan tenido casos de PFA en el 2023. Para los municipios con &lt;100000 menores de 15 años y que no tuvieron casos de PFA en 2023, la celda cambiará a gris y no es necesario completar ninguna información. </t>
+  </si>
+  <si>
+    <t>Esta celda solo debe completarse para los municipios con &lt;100000 menores de 15 años y que no hayan tenido casos de PFA en el 2023</t>
+  </si>
+  <si>
+    <t>Si el país llevó a cabo una campaña de vacunación contra la polio en 2019-2023, ¿se alcanzó una cobertura &gt;95% en el municipio?</t>
+  </si>
+  <si>
+    <t>En los municipios con &lt;100000 menores de 15 años y que no presentaron casos de PFA, ¿se llevaron a cabo búsquedas activas institucionales en al menos un establecimiento de salud del municipio?</t>
+  </si>
+  <si>
+    <t>Si la población &lt;15 años de edad es &lt;100000, ¿se presentaron casos de PFA en el 2023?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">% de unidades notificadoras que enviaron información en todas las semanas durante el periodo evaluado </t>
   </si>
 </sst>
 </file>
@@ -885,7 +888,7 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1051,12 +1054,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="5" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1428,14 +1425,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18904028-F9F6-3046-9356-B730934F1CDF}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="56.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1443,23 +1442,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3">
-        <v>2023</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -1467,17 +1462,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" s="2">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2"/>
     </row>
@@ -1488,6 +1481,18 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BC92D02-843F-244F-9460-E090EF2C7C0A}">
+          <x14:formula1>
+            <xm:f>_ListValues!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>B6</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1495,11 +1500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACD1E9FE-E77B-E547-ADE0-516025CB78C4}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" customWidth="1"/>
@@ -1511,7 +1514,7 @@
     <col min="8" max="8" width="15.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="44" t="s">
         <v>7</v>
       </c>
@@ -1525,19 +1528,19 @@
         <v>10</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="45"/>
       <c r="B2" s="45"/>
       <c r="C2" s="5"/>
@@ -1547,7 +1550,7 @@
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="45"/>
       <c r="C3" s="5"/>
@@ -1557,7 +1560,7 @@
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="5"/>
@@ -1567,7 +1570,7 @@
       <c r="G4" s="7"/>
       <c r="H4" s="7"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="45"/>
       <c r="C5" s="5"/>
@@ -1577,7 +1580,7 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="45"/>
       <c r="B6" s="45"/>
       <c r="C6" s="5"/>
@@ -1587,7 +1590,7 @@
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="45"/>
       <c r="C7" s="5"/>
@@ -1606,11 +1609,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87362FD8-F1C8-0142-963D-AD6273C5898D}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="2" width="16.83203125" customWidth="1"/>
@@ -1618,11 +1621,10 @@
     <col min="4" max="4" width="20.5" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="14.83203125" customWidth="1"/>
-    <col min="12" max="12" width="22.1640625" customWidth="1"/>
-    <col min="13" max="13" width="30.33203125" customWidth="1"/>
+    <col min="9" max="13" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>7</v>
       </c>
@@ -1636,16 +1638,16 @@
         <v>10</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="54" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="I1" s="50" t="s">
         <v>12</v>
@@ -1655,13 +1657,13 @@
       <c r="L1" s="50"/>
       <c r="M1" s="50"/>
       <c r="N1" s="50" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="O1" s="50" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="42" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
       <c r="C2" s="57"/>
@@ -1671,24 +1673,24 @@
       <c r="G2" s="53"/>
       <c r="H2" s="55"/>
       <c r="I2" s="43">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="J2" s="43">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="K2" s="43">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="L2" s="43">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="M2" s="43">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="N2" s="51"/>
       <c r="O2" s="51"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="45"/>
       <c r="C3" s="2"/>
@@ -1705,7 +1707,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="2"/>
@@ -1722,7 +1724,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="45"/>
       <c r="C5" s="2"/>
@@ -1739,7 +1741,7 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="45"/>
       <c r="B6" s="45"/>
       <c r="C6" s="2"/>
@@ -1756,7 +1758,7 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="45"/>
       <c r="C7" s="2"/>
@@ -1773,7 +1775,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="45"/>
       <c r="B8" s="45"/>
       <c r="C8" s="2"/>
@@ -1820,11 +1822,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A24FC60A-8114-B04C-B5D4-941061AFF1F9}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.83203125" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" customWidth="1"/>
@@ -1835,7 +1837,7 @@
     <col min="15" max="15" width="32.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="64" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>7</v>
       </c>
@@ -1849,32 +1851,32 @@
         <v>10</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="54" t="s">
-        <v>45</v>
+        <v>99</v>
       </c>
       <c r="I1" s="46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J1" s="58" t="s">
-        <v>17</v>
+        <v>87</v>
       </c>
       <c r="K1" s="59"/>
       <c r="L1" s="59"/>
       <c r="M1" s="59"/>
       <c r="N1" s="59"/>
       <c r="O1" s="46" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="91" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="91" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
       <c r="C2" s="57"/>
@@ -1884,28 +1886,28 @@
       <c r="G2" s="53"/>
       <c r="H2" s="55"/>
       <c r="I2" s="46" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" s="46" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="46" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="46" t="s">
+      <c r="M2" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="46" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="46" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="46" t="s">
-        <v>22</v>
-      </c>
       <c r="O2" s="46" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="45"/>
       <c r="C3" s="2"/>
@@ -1922,7 +1924,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="2"/>
@@ -1939,7 +1941,7 @@
       <c r="N4" s="8"/>
       <c r="O4" s="8"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="45"/>
       <c r="C5" s="2"/>
@@ -1956,7 +1958,7 @@
       <c r="N5" s="8"/>
       <c r="O5" s="8"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="45"/>
       <c r="B6" s="45"/>
       <c r="C6" s="2"/>
@@ -1973,7 +1975,7 @@
       <c r="N6" s="8"/>
       <c r="O6" s="8"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="45"/>
       <c r="C7" s="2"/>
@@ -1990,7 +1992,7 @@
       <c r="N7" s="8"/>
       <c r="O7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="45"/>
       <c r="B8" s="45"/>
       <c r="C8" s="2"/>
@@ -2036,17 +2038,17 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:G1048576"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="20.83203125" customWidth="1"/>
     <col min="5" max="7" width="12.83203125" customWidth="1"/>
     <col min="8" max="10" width="20.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>7</v>
       </c>
@@ -2060,25 +2062,25 @@
         <v>10</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="60" t="s">
-        <v>45</v>
+      <c r="H1" s="54" t="s">
+        <v>99</v>
       </c>
       <c r="I1" s="48" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J1" s="48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
       <c r="C2" s="57"/>
@@ -2086,15 +2088,15 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="61"/>
+      <c r="H2" s="55"/>
       <c r="I2" s="48" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="J2" s="48" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="45"/>
       <c r="C3" s="2"/>
@@ -2106,7 +2108,7 @@
       <c r="I3" s="8"/>
       <c r="J3" s="8"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="2"/>
@@ -2118,7 +2120,7 @@
       <c r="I4" s="8"/>
       <c r="J4" s="8"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="45"/>
       <c r="C5" s="2"/>
@@ -2130,7 +2132,7 @@
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="45"/>
       <c r="B6" s="45"/>
       <c r="C6" s="2"/>
@@ -2142,7 +2144,7 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="45"/>
       <c r="C7" s="2"/>
@@ -2154,7 +2156,7 @@
       <c r="I7" s="8"/>
       <c r="J7" s="8"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="45"/>
       <c r="B8" s="45"/>
       <c r="C8" s="2"/>
@@ -2193,11 +2195,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5205DBED-7CB8-CA49-87DC-8975752A1842}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="7" width="13.83203125" customWidth="1"/>
@@ -2205,7 +2207,7 @@
     <col min="9" max="9" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="56" t="s">
         <v>7</v>
       </c>
@@ -2219,27 +2221,27 @@
         <v>10</v>
       </c>
       <c r="E1" s="52" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="F1" s="52" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="G1" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="62" t="s">
-        <v>29</v>
-      </c>
-      <c r="J1" s="63"/>
-      <c r="K1" s="63"/>
-      <c r="L1" s="63"/>
-      <c r="M1" s="63"/>
-      <c r="N1" s="63"/>
-    </row>
-    <row r="2" spans="1:14" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H1" s="54" t="s">
+        <v>99</v>
+      </c>
+      <c r="I1" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+    </row>
+    <row r="2" spans="1:14" ht="49" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="56"/>
       <c r="B2" s="56"/>
       <c r="C2" s="57"/>
@@ -2247,27 +2249,27 @@
       <c r="E2" s="53"/>
       <c r="F2" s="53"/>
       <c r="G2" s="53"/>
-      <c r="H2" s="61"/>
+      <c r="H2" s="55"/>
       <c r="I2" s="47" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="J2" s="47" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="K2" s="47" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="L2" s="47" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="M2" s="47" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="N2" s="47" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="45"/>
       <c r="B3" s="45"/>
       <c r="C3" s="2"/>
@@ -2283,7 +2285,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="45"/>
       <c r="B4" s="45"/>
       <c r="C4" s="2"/>
@@ -2299,7 +2301,7 @@
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="45"/>
       <c r="B5" s="45"/>
       <c r="C5" s="2"/>
@@ -2315,7 +2317,7 @@
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="45"/>
       <c r="B6" s="45"/>
       <c r="C6" s="2"/>
@@ -2331,7 +2333,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="45"/>
       <c r="B7" s="45"/>
       <c r="C7" s="2"/>
@@ -2347,7 +2349,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="45"/>
       <c r="B8" s="45"/>
       <c r="C8" s="2"/>
@@ -2381,6 +2383,18 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{68DF49D3-C92F-7E44-81A6-4E0F166AA1B2}">
+          <x14:formula1>
+            <xm:f>_ListValues!$B$2:$B$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>H3:H8</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2388,11 +2402,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24261340-693F-D844-8FDC-79D93DCEE3FF}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="23.5" style="42" customWidth="1"/>
@@ -2401,26 +2415,26 @@
     <col min="5" max="5" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="72" t="s">
-        <v>82</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="70" t="s">
+        <v>66</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>7</v>
@@ -2429,8 +2443,8 @@
       <c r="D2" s="22"/>
       <c r="E2" s="23"/>
     </row>
-    <row r="3" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="73"/>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="71"/>
       <c r="B3" s="39" t="s">
         <v>8</v>
       </c>
@@ -2438,340 +2452,340 @@
       <c r="D3" s="24"/>
       <c r="E3" s="25"/>
     </row>
-    <row r="4" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A4" s="73"/>
+    <row r="4" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="71"/>
       <c r="B4" s="32" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D4" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E4" s="25"/>
     </row>
-    <row r="5" spans="1:5" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="73"/>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="71"/>
       <c r="B5" s="39" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E5" s="25"/>
     </row>
-    <row r="6" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="74"/>
+    <row r="6" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="72"/>
       <c r="B6" s="40" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E6" s="49"/>
     </row>
-    <row r="7" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="74"/>
+    <row r="7" spans="1:5" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="72"/>
       <c r="B7" s="40" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D7" s="27" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E7" s="49"/>
     </row>
-    <row r="8" spans="1:5" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="75"/>
+    <row r="8" spans="1:5" ht="31.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="73"/>
       <c r="B8" s="40" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="26"/>
+    </row>
+    <row r="9" spans="1:5" ht="62" x14ac:dyDescent="0.35">
+      <c r="A9" s="74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="29" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="75"/>
+      <c r="B10" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="16"/>
+    </row>
+    <row r="11" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="75"/>
+      <c r="B11" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="87.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="76"/>
+      <c r="B12" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="27" t="s">
+    </row>
+    <row r="13" spans="1:5" ht="58" x14ac:dyDescent="0.35">
+      <c r="A13" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="26"/>
-    </row>
-    <row r="9" spans="1:5" ht="85" x14ac:dyDescent="0.2">
-      <c r="A9" s="76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="11" t="s">
+      <c r="B13" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="D13" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="28" t="s">
+    </row>
+    <row r="14" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A14" s="63"/>
+      <c r="B14" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="C14" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A15" s="63"/>
+      <c r="B15" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="17" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A10" s="77"/>
-      <c r="B10" s="17" t="s">
+      <c r="D15" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A16" s="63"/>
+      <c r="B16" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="17" t="s">
+      <c r="D16" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A17" s="63"/>
+      <c r="B17" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="E10" s="16"/>
-    </row>
-    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A11" s="77"/>
-      <c r="B11" s="17" t="s">
+      <c r="C17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D17" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="A18" s="63"/>
+      <c r="B18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="D11" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E11" s="18" t="s">
+      <c r="D18" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="116.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="64"/>
+      <c r="B19" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="33" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="78"/>
-      <c r="B12" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="20" t="s">
+      <c r="D19" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="34" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="145" x14ac:dyDescent="0.35">
+      <c r="A20" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="D12" s="20" t="s">
+      <c r="B20" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="31" t="s">
+      <c r="D20" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A13" s="64" t="s">
+    <row r="21" spans="1:5" ht="102" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="66"/>
+      <c r="B21" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="17" t="s">
+      <c r="D21" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="B22" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="18" t="s">
+      <c r="D22" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E22" s="14"/>
+    </row>
+    <row r="23" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="68"/>
+      <c r="B23" s="36" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A14" s="65"/>
-      <c r="B14" s="17" t="s">
+      <c r="C23" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C14" s="17" t="s">
+      <c r="D23" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="16"/>
+    </row>
+    <row r="24" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="68"/>
+      <c r="B24" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="D24" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+      <c r="A25" s="68"/>
+      <c r="B25" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A15" s="65"/>
-      <c r="B15" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="17" t="s">
+      <c r="D25" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="16"/>
+    </row>
+    <row r="26" spans="1:5" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A26" s="69"/>
+      <c r="B26" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A16" s="65"/>
-      <c r="B16" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="17" t="s">
+      <c r="C26" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A17" s="65"/>
-      <c r="B17" s="17" t="s">
+      <c r="D26" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="21"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="13" t="s">
         <v>65</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="96" x14ac:dyDescent="0.2">
-      <c r="A18" s="65"/>
-      <c r="B18" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
-      <c r="B19" s="33" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="33" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="34" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="160" x14ac:dyDescent="0.2">
-      <c r="A20" s="67" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="97" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="68"/>
-      <c r="B21" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="31" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A22" s="69" t="s">
-        <v>84</v>
-      </c>
-      <c r="B22" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="70"/>
-      <c r="B23" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="16"/>
-    </row>
-    <row r="24" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="70"/>
-      <c r="B24" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>77</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="16"/>
-    </row>
-    <row r="25" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A25" s="70"/>
-      <c r="B25" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C25" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="E25" s="16"/>
-    </row>
-    <row r="26" spans="1:5" ht="33" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
-      <c r="B26" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="C26" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="D26" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="21"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="13" t="s">
-        <v>81</v>
       </c>
       <c r="B27" s="41"/>
       <c r="C27" s="13"/>
@@ -2795,62 +2809,62 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>88</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>74</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>